<commit_message>
Added local errors, fixed test case
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="141">
   <si>
     <t>Name</t>
   </si>
@@ -463,6 +463,12 @@
   </si>
   <si>
     <t>Dispatcher</t>
+  </si>
+  <si>
+    <t>ErrorCodePath</t>
+  </si>
+  <si>
+    <t>Data\ErrorCodes.xlsx</t>
   </si>
 </sst>
 </file>
@@ -864,7 +870,7 @@
   <dimension ref="A1:Z1012"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1136,7 +1142,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" t="s">
+        <v>140</v>
+      </c>
+    </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>

</xml_diff>